<commit_message>
update the server proxy
</commit_message>
<xml_diff>
--- a/docs/server-proxy.xlsx
+++ b/docs/server-proxy.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
   <si>
     <t>type</t>
   </si>
@@ -77,6 +77,9 @@
     <t>文件/信息</t>
   </si>
   <si>
+    <t>状态</t>
+  </si>
+  <si>
     <t>0000</t>
   </si>
   <si>
@@ -105,6 +108,27 @@
   </si>
   <si>
     <t>获取用户好友</t>
+  </si>
+  <si>
+    <t>0005</t>
+  </si>
+  <si>
+    <t>添加好友</t>
+  </si>
+  <si>
+    <t>两个</t>
+  </si>
+  <si>
+    <t>0006</t>
+  </si>
+  <si>
+    <t>处理请求</t>
+  </si>
+  <si>
+    <t>0007</t>
+  </si>
+  <si>
+    <t>添加好友的通知</t>
   </si>
 </sst>
 </file>
@@ -720,24 +744,30 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1275,20 +1305,21 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:U7"/>
+  <dimension ref="A1:V10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2"/>
+    <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" workbookViewId="0">
+      <selection activeCell="U5" sqref="U5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.81818181818182" defaultRowHeight="14" outlineLevelRow="6"/>
+  <sheetFormatPr defaultColWidth="9.81818181818182" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="9.81818181818182" style="1"/>
     <col min="2" max="2" width="16.2727272727273" style="1" customWidth="1"/>
     <col min="3" max="20" width="9.81818181818182" style="1"/>
+    <col min="21" max="22" width="9.81818181818182" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:22">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1302,8 +1333,9 @@
         <v>3</v>
       </c>
       <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
     </row>
-    <row r="2" spans="3:21">
+    <row r="2" spans="3:22">
       <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
@@ -1358,79 +1390,127 @@
       <c r="T2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="U2" s="4" t="s">
+      <c r="U2" s="5" t="s">
         <v>7</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" s="6" t="s">
-        <v>16</v>
+      <c r="A3" s="8" t="s">
+        <v>17</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="3"/>
+        <v>18</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="4"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="6" t="s">
-        <v>18</v>
+      <c r="A4" s="8" t="s">
+        <v>19</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+        <v>20</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
     </row>
     <row r="5" spans="1:21">
-      <c r="A5" s="6" t="s">
-        <v>20</v>
+      <c r="A5" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
-      <c r="S5" s="2"/>
-      <c r="T5" s="2"/>
-      <c r="U5" s="5"/>
+        <v>22</v>
+      </c>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="6"/>
     </row>
-    <row r="6" spans="1:21">
-      <c r="A6" s="6" t="s">
-        <v>22</v>
+    <row r="6" spans="1:22">
+      <c r="A6" s="8" t="s">
+        <v>23</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-      <c r="S6" s="2"/>
-      <c r="T6" s="2"/>
-      <c r="U6" s="5"/>
+        <v>24</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="M6" s="3">
+        <v>1</v>
+      </c>
+      <c r="N6" s="3">
+        <v>2</v>
+      </c>
+      <c r="O6" s="3">
+        <v>5</v>
+      </c>
+      <c r="S6" s="3">
+        <v>3</v>
+      </c>
+      <c r="T6" s="3">
+        <v>4</v>
+      </c>
+      <c r="U6" s="7"/>
+      <c r="V6" s="6">
+        <v>6</v>
+      </c>
     </row>
     <row r="7" spans="1:17">
-      <c r="A7" s="6" t="s">
-        <v>24</v>
+      <c r="A7" s="8" t="s">
+        <v>25</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="2"/>
-      <c r="Q7" s="2"/>
+        <v>26</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="Q7" s="3"/>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="M10" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="C1:L1"/>
-    <mergeCell ref="M1:U1"/>
+    <mergeCell ref="M1:V1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
   </mergeCells>

</xml_diff>

<commit_message>
add get user status in group
</commit_message>
<xml_diff>
--- a/docs/server-proxy.xlsx
+++ b/docs/server-proxy.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="77">
   <si>
     <t>type</t>
   </si>
@@ -249,6 +249,15 @@
   </si>
   <si>
     <t>3:退出</t>
+  </si>
+  <si>
+    <t>0019</t>
+  </si>
+  <si>
+    <t>获取用户与群聊状态码</t>
+  </si>
+  <si>
+    <t>状态码</t>
   </si>
 </sst>
 </file>
@@ -870,7 +879,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -881,6 +890,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1422,10 +1434,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:V21"/>
+  <dimension ref="A1:V22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+    <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.81818181818182" defaultRowHeight="14"/>
@@ -1514,7 +1526,7 @@
       </c>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1529,7 +1541,7 @@
       <c r="M3" s="4"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="6" t="s">
         <v>19</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1540,7 +1552,7 @@
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:21">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="6" t="s">
         <v>21</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1554,7 +1566,7 @@
       <c r="U5" s="2"/>
     </row>
     <row r="6" spans="1:22">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="6" t="s">
         <v>23</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1582,7 +1594,7 @@
       </c>
     </row>
     <row r="7" spans="1:17">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="6" t="s">
         <v>25</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1592,7 +1604,7 @@
       <c r="Q7" s="2"/>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="6" t="s">
         <v>27</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1603,7 +1615,7 @@
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="6" t="s">
         <v>30</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1614,7 +1626,7 @@
       </c>
     </row>
     <row r="10" spans="1:13">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="6" t="s">
         <v>32</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1624,7 +1636,7 @@
       <c r="M10" s="2"/>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="6" t="s">
         <v>34</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -1635,7 +1647,7 @@
       </c>
     </row>
     <row r="12" spans="1:12">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="6" t="s">
         <v>36</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1648,7 +1660,7 @@
       <c r="L12" s="2"/>
     </row>
     <row r="13" spans="1:18">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="6" t="s">
         <v>38</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -1662,7 +1674,7 @@
       </c>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="6" t="s">
         <v>41</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1674,7 +1686,7 @@
       <c r="I14" s="2"/>
     </row>
     <row r="15" spans="1:16">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="6" t="s">
         <v>43</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -1697,7 +1709,7 @@
       </c>
     </row>
     <row r="16" spans="1:13">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="6" t="s">
         <v>49</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -1711,7 +1723,7 @@
       </c>
     </row>
     <row r="17" spans="1:15">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="6" t="s">
         <v>52</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -1731,7 +1743,7 @@
       </c>
     </row>
     <row r="18" spans="1:13">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="6" t="s">
         <v>56</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -1746,12 +1758,10 @@
       <c r="E18" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="M18" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="5" t="s">
+      <c r="M18" s="5"/>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" s="6" t="s">
         <v>59</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -1766,9 +1776,10 @@
       <c r="E19" s="3" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="5" t="s">
+      <c r="M19" s="5"/>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20" s="6" t="s">
         <v>63</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -1789,9 +1800,12 @@
       <c r="G20" s="1" t="s">
         <v>68</v>
       </c>
+      <c r="M20" s="3" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="6" t="s">
         <v>69</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -1814,6 +1828,23 @@
       </c>
       <c r="H21" s="1" t="s">
         <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="M22" s="3" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>